<commit_message>
Add Skylab 1 saturn masses, fix LEB DSKy lighting in VC
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F99C9B-F8F6-4CDF-B8C5-053851B2E4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC89749-DE31-4210-8970-D2E3798A348E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="Apollo 8" sheetId="4" r:id="rId10"/>
     <sheet name="Apollo 7" sheetId="13" r:id="rId11"/>
     <sheet name="Apollo 5" sheetId="16" r:id="rId12"/>
-    <sheet name="Totals" sheetId="14" r:id="rId13"/>
+    <sheet name="Skylab 1" sheetId="18" r:id="rId13"/>
+    <sheet name="Skylab 2" sheetId="17" r:id="rId14"/>
+    <sheet name="Totals" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7693" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8545" uniqueCount="159">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -386,9 +388,6 @@
     <t>S-IB Retromotor Prop</t>
   </si>
   <si>
-    <t>Data From Saturn S-IVB-505 Stage Flight Evaluation Report &amp; Launch Vehicle Evaluation Report</t>
-  </si>
-  <si>
     <t>Apollo 7</t>
   </si>
   <si>
@@ -495,6 +494,39 @@
   </si>
   <si>
     <t>S-IVB</t>
+  </si>
+  <si>
+    <t>Data From Saturn S-IVB Stage Flight Evaluation Report &amp; Launch Vehicle Evaluation Report</t>
+  </si>
+  <si>
+    <t>Data From Launch Vehicle Evaluation Report</t>
+  </si>
+  <si>
+    <t>Total S-II/OWS IS</t>
+  </si>
+  <si>
+    <t>S-II/OWS SEP</t>
+  </si>
+  <si>
+    <t>OWSMASS</t>
+  </si>
+  <si>
+    <t>OWS</t>
+  </si>
+  <si>
+    <t>OWS Met Shield</t>
+  </si>
+  <si>
+    <t>OWS Aft Frame</t>
+  </si>
+  <si>
+    <t>OWS Det Pkg</t>
+  </si>
+  <si>
+    <t>Skylab In Orbit</t>
+  </si>
+  <si>
+    <t>OWSMETSHLD</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4B85CD-0950-475D-8BA8-941ABAD25001}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7153,8 +7185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80FCE58-7FB9-4CC7-8163-D01D25C81D7D}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10264,7 +10296,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -10281,8 +10313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8612F4-CCB1-4696-8897-C4C5EFBE3F4E}">
   <dimension ref="A1:AV39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10367,19 +10399,19 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
@@ -10397,7 +10429,7 @@
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
@@ -10414,7 +10446,7 @@
       </c>
       <c r="E2" s="24"/>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2">
         <v>10649</v>
@@ -10424,7 +10456,7 @@
       </c>
       <c r="I2" s="24"/>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K2">
         <v>10649</v>
@@ -10434,7 +10466,7 @@
       </c>
       <c r="M2" s="24"/>
       <c r="N2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O2">
         <v>10649</v>
@@ -10444,7 +10476,7 @@
       </c>
       <c r="Q2" s="24"/>
       <c r="R2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S2">
         <v>10649</v>
@@ -10454,7 +10486,7 @@
       </c>
       <c r="U2" s="24"/>
       <c r="V2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W2">
         <v>10649</v>
@@ -10464,7 +10496,7 @@
       </c>
       <c r="Y2" s="24"/>
       <c r="Z2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AA2">
         <v>10649</v>
@@ -10474,7 +10506,7 @@
       </c>
       <c r="AC2" s="24"/>
       <c r="AD2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE2">
         <v>10649</v>
@@ -10484,7 +10516,7 @@
       </c>
       <c r="AG2" s="24"/>
       <c r="AH2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AI2">
         <v>10649</v>
@@ -10494,7 +10526,7 @@
       </c>
       <c r="AK2" s="24"/>
       <c r="AL2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AM2">
         <v>10649</v>
@@ -10504,7 +10536,7 @@
       </c>
       <c r="AO2" s="24"/>
       <c r="AP2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AQ2">
         <v>10649</v>
@@ -10514,7 +10546,7 @@
       </c>
       <c r="AS2" s="24"/>
       <c r="AT2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AU2">
         <v>10649</v>
@@ -10585,7 +10617,7 @@
       </c>
       <c r="Y3" s="24"/>
       <c r="Z3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA3">
         <v>1135.8</v>
@@ -10595,7 +10627,7 @@
       </c>
       <c r="AC3" s="24"/>
       <c r="AD3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AE3">
         <v>1122.5999999999999</v>
@@ -10605,7 +10637,7 @@
       </c>
       <c r="AG3" s="24"/>
       <c r="AH3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AI3">
         <v>1075.4000000000001</v>
@@ -10615,7 +10647,7 @@
       </c>
       <c r="AK3" s="24"/>
       <c r="AL3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AM3">
         <v>946.2</v>
@@ -10625,7 +10657,7 @@
       </c>
       <c r="AO3" s="24"/>
       <c r="AP3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AQ3">
         <v>0</v>
@@ -10635,7 +10667,7 @@
       </c>
       <c r="AS3" s="24"/>
       <c r="AT3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AU3">
         <v>0</v>
@@ -10656,7 +10688,7 @@
       </c>
       <c r="E4" s="24"/>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4">
         <v>100.7</v>
@@ -10666,7 +10698,7 @@
       </c>
       <c r="I4" s="24"/>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K4">
         <v>100.7</v>
@@ -10676,7 +10708,7 @@
       </c>
       <c r="M4" s="24"/>
       <c r="N4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O4">
         <v>100.7</v>
@@ -10686,7 +10718,7 @@
       </c>
       <c r="Q4" s="24"/>
       <c r="R4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -10696,7 +10728,7 @@
       </c>
       <c r="U4" s="24"/>
       <c r="V4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -10777,7 +10809,7 @@
       </c>
       <c r="E5" s="24"/>
       <c r="F5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5">
         <v>80.3</v>
@@ -10787,7 +10819,7 @@
       </c>
       <c r="I5" s="24"/>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K5">
         <v>45.4</v>
@@ -10797,7 +10829,7 @@
       </c>
       <c r="M5" s="24"/>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -10807,7 +10839,7 @@
       </c>
       <c r="Q5" s="24"/>
       <c r="R5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -10817,7 +10849,7 @@
       </c>
       <c r="U5" s="24"/>
       <c r="V5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -10898,7 +10930,7 @@
       </c>
       <c r="E6" s="24"/>
       <c r="F6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6">
         <v>87862.2</v>
@@ -10908,7 +10940,7 @@
       </c>
       <c r="I6" s="24"/>
       <c r="J6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K6">
         <v>87859.9</v>
@@ -10918,7 +10950,7 @@
       </c>
       <c r="M6" s="24"/>
       <c r="N6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O6">
         <v>87397.2</v>
@@ -10928,7 +10960,7 @@
       </c>
       <c r="Q6" s="24"/>
       <c r="R6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S6">
         <v>1197.9000000000001</v>
@@ -10938,7 +10970,7 @@
       </c>
       <c r="U6" s="24"/>
       <c r="V6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W6">
         <v>1143.5</v>
@@ -10948,7 +10980,7 @@
       </c>
       <c r="Y6" s="24"/>
       <c r="Z6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AA6">
         <v>624.20000000000005</v>
@@ -10958,7 +10990,7 @@
       </c>
       <c r="AC6" s="24"/>
       <c r="AD6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AE6">
         <v>484</v>
@@ -10968,7 +11000,7 @@
       </c>
       <c r="AG6" s="24"/>
       <c r="AH6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AI6">
         <v>155.6</v>
@@ -10978,7 +11010,7 @@
       </c>
       <c r="AK6" s="24"/>
       <c r="AL6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -10988,7 +11020,7 @@
       </c>
       <c r="AO6" s="24"/>
       <c r="AP6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AQ6">
         <v>0</v>
@@ -10998,7 +11030,7 @@
       </c>
       <c r="AS6" s="24"/>
       <c r="AT6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AU6">
         <v>0</v>
@@ -11261,7 +11293,7 @@
       </c>
       <c r="E9" s="24"/>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G9">
         <v>16903.599999999999</v>
@@ -11271,7 +11303,7 @@
       </c>
       <c r="I9" s="24"/>
       <c r="J9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K9">
         <v>16894.5</v>
@@ -11281,7 +11313,7 @@
       </c>
       <c r="M9" s="24"/>
       <c r="N9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O9">
         <v>16773.400000000001</v>
@@ -11291,7 +11323,7 @@
       </c>
       <c r="Q9" s="24"/>
       <c r="R9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S9">
         <v>647.29999999999995</v>
@@ -11301,7 +11333,7 @@
       </c>
       <c r="U9" s="24"/>
       <c r="V9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="W9">
         <v>635</v>
@@ -11311,7 +11343,7 @@
       </c>
       <c r="Y9" s="24"/>
       <c r="Z9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA9">
         <v>71.2</v>
@@ -11321,7 +11353,7 @@
       </c>
       <c r="AC9" s="24"/>
       <c r="AD9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AE9">
         <v>71.2</v>
@@ -11331,7 +11363,7 @@
       </c>
       <c r="AG9" s="24"/>
       <c r="AH9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AI9">
         <v>71.2</v>
@@ -11341,7 +11373,7 @@
       </c>
       <c r="AK9" s="24"/>
       <c r="AL9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AM9">
         <v>71.2</v>
@@ -11351,7 +11383,7 @@
       </c>
       <c r="AO9" s="24"/>
       <c r="AP9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AQ9">
         <v>71.2</v>
@@ -11361,7 +11393,7 @@
       </c>
       <c r="AS9" s="24"/>
       <c r="AT9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AU9">
         <v>0</v>
@@ -11624,7 +11656,7 @@
       </c>
       <c r="E12" s="24"/>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G12">
         <v>143.30000000000001</v>
@@ -11634,7 +11666,7 @@
       </c>
       <c r="I12" s="24"/>
       <c r="J12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K12">
         <v>143.30000000000001</v>
@@ -11644,7 +11676,7 @@
       </c>
       <c r="M12" s="24"/>
       <c r="N12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O12">
         <v>142.9</v>
@@ -11654,7 +11686,7 @@
       </c>
       <c r="Q12" s="24"/>
       <c r="R12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S12">
         <v>71.2</v>
@@ -11664,7 +11696,7 @@
       </c>
       <c r="U12" s="24"/>
       <c r="V12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W12">
         <v>71.2</v>
@@ -11674,7 +11706,7 @@
       </c>
       <c r="Y12" s="24"/>
       <c r="Z12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AA12">
         <v>3.2</v>
@@ -11684,7 +11716,7 @@
       </c>
       <c r="AC12" s="24"/>
       <c r="AD12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AE12">
         <v>3.2</v>
@@ -11694,7 +11726,7 @@
       </c>
       <c r="AG12" s="24"/>
       <c r="AH12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AI12">
         <v>3.2</v>
@@ -11704,7 +11736,7 @@
       </c>
       <c r="AK12" s="24"/>
       <c r="AL12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AM12">
         <v>3.2</v>
@@ -11714,7 +11746,7 @@
       </c>
       <c r="AO12" s="24"/>
       <c r="AP12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AQ12">
         <v>3.2</v>
@@ -11724,7 +11756,7 @@
       </c>
       <c r="AS12" s="24"/>
       <c r="AT12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AU12">
         <v>3.2</v>
@@ -11795,7 +11827,7 @@
       </c>
       <c r="Y13" s="24"/>
       <c r="Z13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AA13">
         <v>19.5</v>
@@ -11805,7 +11837,7 @@
       </c>
       <c r="AC13" s="24"/>
       <c r="AD13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AE13">
         <v>19.5</v>
@@ -11815,7 +11847,7 @@
       </c>
       <c r="AG13" s="24"/>
       <c r="AH13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AI13">
         <v>19.5</v>
@@ -11825,7 +11857,7 @@
       </c>
       <c r="AK13" s="24"/>
       <c r="AL13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AM13">
         <v>19.5</v>
@@ -11835,7 +11867,7 @@
       </c>
       <c r="AO13" s="24"/>
       <c r="AP13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AQ13">
         <v>19.5</v>
@@ -11845,7 +11877,7 @@
       </c>
       <c r="AS13" s="24"/>
       <c r="AT13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AU13">
         <v>19.5</v>
@@ -11985,7 +12017,7 @@
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="E15" s="24"/>
       <c r="F15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G15">
         <v>2.2000000000000002</v>
@@ -11995,7 +12027,7 @@
       </c>
       <c r="I15" s="24"/>
       <c r="J15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K15">
         <v>2.2000000000000002</v>
@@ -12005,7 +12037,7 @@
       </c>
       <c r="M15" s="24"/>
       <c r="N15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O15">
         <v>0.5</v>
@@ -12015,7 +12047,7 @@
       </c>
       <c r="Q15" s="24"/>
       <c r="R15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S15">
         <v>3.2</v>
@@ -12025,7 +12057,7 @@
       </c>
       <c r="U15" s="24"/>
       <c r="V15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W15">
         <v>3.2</v>
@@ -12106,7 +12138,7 @@
       </c>
       <c r="E16" s="24"/>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G16">
         <v>19.5</v>
@@ -12116,7 +12148,7 @@
       </c>
       <c r="I16" s="24"/>
       <c r="J16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K16">
         <v>19.5</v>
@@ -12126,7 +12158,7 @@
       </c>
       <c r="M16" s="24"/>
       <c r="N16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O16">
         <v>19.5</v>
@@ -12136,7 +12168,7 @@
       </c>
       <c r="Q16" s="24"/>
       <c r="R16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S16">
         <v>19.5</v>
@@ -12146,7 +12178,7 @@
       </c>
       <c r="U16" s="24"/>
       <c r="V16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W16">
         <v>19.5</v>
@@ -12156,7 +12188,7 @@
       </c>
       <c r="Y16" s="24"/>
       <c r="Z16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AA16">
         <v>1750.4</v>
@@ -12166,7 +12198,7 @@
       </c>
       <c r="AC16" s="24"/>
       <c r="AD16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AE16">
         <v>1750.4</v>
@@ -12176,7 +12208,7 @@
       </c>
       <c r="AG16" s="24"/>
       <c r="AH16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AI16">
         <v>1750.4</v>
@@ -12186,7 +12218,7 @@
       </c>
       <c r="AK16" s="24"/>
       <c r="AL16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AM16">
         <v>1750.4</v>
@@ -12196,7 +12228,7 @@
       </c>
       <c r="AO16" s="24"/>
       <c r="AP16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AQ16">
         <v>1750.4</v>
@@ -12206,7 +12238,7 @@
       </c>
       <c r="AS16" s="24"/>
       <c r="AT16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AU16">
         <v>1750.4</v>
@@ -12277,7 +12309,7 @@
       </c>
       <c r="Y17" s="24"/>
       <c r="Z17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AA17">
         <v>14301.7</v>
@@ -12287,7 +12319,7 @@
       </c>
       <c r="AC17" s="24"/>
       <c r="AD17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AE17">
         <v>14301.7</v>
@@ -12297,7 +12329,7 @@
       </c>
       <c r="AG17" s="24"/>
       <c r="AH17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AI17">
         <v>0</v>
@@ -12307,7 +12339,7 @@
       </c>
       <c r="AK17" s="24"/>
       <c r="AL17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AM17">
         <v>0</v>
@@ -12317,7 +12349,7 @@
       </c>
       <c r="AO17" s="24"/>
       <c r="AP17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AQ17">
         <v>0</v>
@@ -12327,7 +12359,7 @@
       </c>
       <c r="AS17" s="24"/>
       <c r="AT17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AU17">
         <v>0</v>
@@ -12539,7 +12571,7 @@
       </c>
       <c r="E20" s="24"/>
       <c r="F20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G20">
         <v>16577.400000000001</v>
@@ -12549,7 +12581,7 @@
       </c>
       <c r="I20" s="24"/>
       <c r="J20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K20">
         <v>16577.400000000001</v>
@@ -12559,7 +12591,7 @@
       </c>
       <c r="M20" s="24"/>
       <c r="N20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O20">
         <v>16577.400000000001</v>
@@ -12569,7 +12601,7 @@
       </c>
       <c r="Q20" s="24"/>
       <c r="R20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S20">
         <v>16577.400000000001</v>
@@ -12579,7 +12611,7 @@
       </c>
       <c r="U20" s="24"/>
       <c r="V20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W20">
         <v>16577.400000000001</v>
@@ -12606,7 +12638,7 @@
       </c>
       <c r="E21" s="24"/>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G21">
         <f>SUM(G18:G20)</f>
@@ -12617,7 +12649,7 @@
       </c>
       <c r="I21" s="24"/>
       <c r="J21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K21">
         <f>SUM(K18:K20)</f>
@@ -12628,7 +12660,7 @@
       </c>
       <c r="M21" s="24"/>
       <c r="N21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O21">
         <f>SUM(O18:O20)</f>
@@ -12639,7 +12671,7 @@
       </c>
       <c r="Q21" s="24"/>
       <c r="R21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S21">
         <f>SUM(S18:S20)</f>
@@ -12650,7 +12682,7 @@
       </c>
       <c r="U21" s="24"/>
       <c r="V21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W21">
         <f>SUM(W18:W20)</f>
@@ -12855,7 +12887,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12869,10 +12901,3595 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14578659-5C6E-4805-8141-DF9DD1CD818C}">
+  <dimension ref="A1:AB42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>130453</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>622</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA2">
+        <v>522</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1480077</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>4985</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3">
+        <v>4985</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3">
+        <v>4985</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3">
+        <v>4985</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3">
+        <v>4985</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA3">
+        <v>21</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>21123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" t="s">
+        <v>30</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>190</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <f>SUM(G2:G4)</f>
+        <v>5607</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <f>SUM(K2:K4)</f>
+        <v>4985</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5">
+        <f>SUM(O2:O4)</f>
+        <v>4985</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5">
+        <f>SUM(S2:S4)</f>
+        <v>4985</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5">
+        <f>SUM(W2:W4)</f>
+        <v>4985</v>
+      </c>
+      <c r="X5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA5">
+        <v>88474</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>633481</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4313</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7">
+        <v>36653</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7">
+        <v>36653</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7">
+        <v>36653</v>
+      </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7">
+        <v>36653</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W7">
+        <v>36653</v>
+      </c>
+      <c r="X7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>372216</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>372216</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>371755</v>
+      </c>
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>7536</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>7407</v>
+      </c>
+      <c r="X8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>737</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>737</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>800</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>787</v>
+      </c>
+      <c r="T9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" t="s">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>787</v>
+      </c>
+      <c r="X9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>288</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>176</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>176</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>179</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>1991</v>
+      </c>
+      <c r="T10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>1996</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>635</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>72695</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11">
+        <v>72689</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>72475</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11">
+        <v>2666</v>
+      </c>
+      <c r="T11" t="s">
+        <v>13</v>
+      </c>
+      <c r="V11" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11">
+        <v>2620</v>
+      </c>
+      <c r="X11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1026</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12">
+        <v>104</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12">
+        <v>110</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12">
+        <v>127</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12">
+        <v>123</v>
+      </c>
+      <c r="T12" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12">
+        <v>123</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>239</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13">
+        <v>38</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13">
+        <v>39</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13">
+        <v>798</v>
+      </c>
+      <c r="T13" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13">
+        <v>800</v>
+      </c>
+      <c r="X13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
+        <v>2271905</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R15" t="s">
+        <v>9</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>13</v>
+      </c>
+      <c r="V15" t="s">
+        <v>9</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>5608</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="R16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16" t="s">
+        <v>13</v>
+      </c>
+      <c r="V16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>482891</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17">
+        <v>34</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="R17" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>34</v>
+      </c>
+      <c r="T17" t="s">
+        <v>13</v>
+      </c>
+      <c r="V17" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17">
+        <v>34</v>
+      </c>
+      <c r="X17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>3453</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <f>SUM(G7:G17)</f>
+        <v>482886</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <f>SUM(K7:K17)</f>
+        <v>482666</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <f>SUM(O7:O17)</f>
+        <v>482064</v>
+      </c>
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18">
+        <f>SUM(S7:S17)</f>
+        <v>50590</v>
+      </c>
+      <c r="T18" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" t="s">
+        <v>15</v>
+      </c>
+      <c r="W18">
+        <f>SUM(W7:W17)</f>
+        <v>50422</v>
+      </c>
+      <c r="X18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>89096</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>581049</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>3453</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20">
+        <v>3453</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" t="s">
+        <v>150</v>
+      </c>
+      <c r="O20">
+        <v>3453</v>
+      </c>
+      <c r="P20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R20" t="s">
+        <v>150</v>
+      </c>
+      <c r="S20">
+        <v>3453</v>
+      </c>
+      <c r="T20" t="s">
+        <v>13</v>
+      </c>
+      <c r="V20" t="s">
+        <v>150</v>
+      </c>
+      <c r="W20">
+        <v>3453</v>
+      </c>
+      <c r="X20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>2852959</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21">
+        <v>89096</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21">
+        <v>88573</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21">
+        <v>88573</v>
+      </c>
+      <c r="P21" t="s">
+        <v>13</v>
+      </c>
+      <c r="R21" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21">
+        <v>88497</v>
+      </c>
+      <c r="T21" t="s">
+        <v>13</v>
+      </c>
+      <c r="V21" t="s">
+        <v>19</v>
+      </c>
+      <c r="W21">
+        <v>88497</v>
+      </c>
+      <c r="X21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>92550</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22">
+        <v>92027</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <v>92027</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+      <c r="R22" t="s">
+        <v>20</v>
+      </c>
+      <c r="S22">
+        <v>91950</v>
+      </c>
+      <c r="T22" t="s">
+        <v>13</v>
+      </c>
+      <c r="V22" t="s">
+        <v>20</v>
+      </c>
+      <c r="W22">
+        <v>91950</v>
+      </c>
+      <c r="X22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>581049</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23">
+        <v>579683</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <v>579081</v>
+      </c>
+      <c r="P23" t="s">
+        <v>13</v>
+      </c>
+      <c r="R23" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23">
+        <v>147530</v>
+      </c>
+      <c r="T23" t="s">
+        <v>13</v>
+      </c>
+      <c r="V23" t="s">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>147363</v>
+      </c>
+      <c r="X23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4">
+        <f>C3+C4+C5+C6+C7+C8</f>
+        <v>2139228</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29">
+        <f>G8+G9+G10+G11+G12+G13</f>
+        <v>445965</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30">
+        <f>AA2</f>
+        <v>522</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31">
+        <f>C2+C9+C10+C12+C13+B37+G2</f>
+        <v>133503</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32">
+        <f>K7+K16+K17+K20</f>
+        <v>40153</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33">
+        <f>AA3+AA4</f>
+        <v>22</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34">
+        <f>AA5</f>
+        <v>88474</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="9">
+        <f>G3</f>
+        <v>4985</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37">
+        <f>C11+G15</f>
+        <v>839</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38">
+        <f>C12</f>
+        <v>1026</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34802A29-2759-43CC-BC11-BE135C5FFFE5}">
+  <dimension ref="A1:AV39"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
+    <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.42578125" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" customWidth="1"/>
+    <col min="28" max="28" width="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.42578125" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.28515625" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" customWidth="1"/>
+    <col min="36" max="36" width="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.85546875" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" customWidth="1"/>
+    <col min="40" max="40" width="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="6.85546875" customWidth="1"/>
+    <col min="42" max="42" width="17.28515625" customWidth="1"/>
+    <col min="44" max="44" width="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.85546875" customWidth="1"/>
+    <col min="46" max="46" width="17.28515625" customWidth="1"/>
+    <col min="48" max="48" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="24"/>
+      <c r="N2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="24"/>
+      <c r="R2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="24"/>
+      <c r="V2" t="s">
+        <v>108</v>
+      </c>
+      <c r="X2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="24"/>
+      <c r="Z2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC2" s="24"/>
+      <c r="AD2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG2" s="24"/>
+      <c r="AH2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK2" s="24"/>
+      <c r="AL2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AO2" s="24"/>
+      <c r="AP2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS2" s="24"/>
+      <c r="AT2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="24"/>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="24"/>
+      <c r="R3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="24"/>
+      <c r="V3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="24"/>
+      <c r="Z3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC3" s="24"/>
+      <c r="AD3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG3" s="24"/>
+      <c r="AH3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK3" s="24"/>
+      <c r="AL3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO3" s="24"/>
+      <c r="AP3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS3" s="24"/>
+      <c r="AT3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="24"/>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="24"/>
+      <c r="V4" t="s">
+        <v>78</v>
+      </c>
+      <c r="X4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="24"/>
+      <c r="Z4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC4" s="24"/>
+      <c r="AD4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG4" s="24"/>
+      <c r="AH4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK4" s="24"/>
+      <c r="AL4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO4" s="24"/>
+      <c r="AP4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS4" s="24"/>
+      <c r="AT4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="24"/>
+      <c r="N5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="24"/>
+      <c r="R5" t="s">
+        <v>79</v>
+      </c>
+      <c r="T5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U5" s="24"/>
+      <c r="V5" t="s">
+        <v>79</v>
+      </c>
+      <c r="X5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" s="24"/>
+      <c r="Z5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC5" s="24"/>
+      <c r="AD5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG5" s="24"/>
+      <c r="AH5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK5" s="24"/>
+      <c r="AL5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO5" s="24"/>
+      <c r="AP5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS5" s="24"/>
+      <c r="AT5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="24"/>
+      <c r="N6" t="s">
+        <v>80</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="24"/>
+      <c r="R6" t="s">
+        <v>80</v>
+      </c>
+      <c r="T6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U6" s="24"/>
+      <c r="V6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="24"/>
+      <c r="Z6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC6" s="24"/>
+      <c r="AD6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG6" s="24"/>
+      <c r="AH6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK6" s="24"/>
+      <c r="AL6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO6" s="24"/>
+      <c r="AP6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS6" s="24"/>
+      <c r="AT6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="24"/>
+      <c r="J7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="24"/>
+      <c r="R7" t="s">
+        <v>81</v>
+      </c>
+      <c r="T7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" s="24"/>
+      <c r="V7" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="24"/>
+      <c r="Z7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="24"/>
+      <c r="AD7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG7" s="24"/>
+      <c r="AH7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK7" s="24"/>
+      <c r="AL7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO7" s="24"/>
+      <c r="AP7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS7" s="24"/>
+      <c r="AT7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="24"/>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="24"/>
+      <c r="R8" t="s">
+        <v>82</v>
+      </c>
+      <c r="T8" t="s">
+        <v>13</v>
+      </c>
+      <c r="U8" s="24"/>
+      <c r="V8" t="s">
+        <v>82</v>
+      </c>
+      <c r="X8" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y8" s="24"/>
+      <c r="Z8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC8" s="24"/>
+      <c r="AD8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG8" s="24"/>
+      <c r="AH8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK8" s="24"/>
+      <c r="AL8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO8" s="24"/>
+      <c r="AP8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS8" s="24"/>
+      <c r="AT8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="24"/>
+      <c r="J9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="24"/>
+      <c r="R9" t="s">
+        <v>83</v>
+      </c>
+      <c r="T9" t="s">
+        <v>13</v>
+      </c>
+      <c r="U9" s="24"/>
+      <c r="V9" t="s">
+        <v>83</v>
+      </c>
+      <c r="X9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y9" s="24"/>
+      <c r="Z9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC9" s="24"/>
+      <c r="AD9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG9" s="24"/>
+      <c r="AH9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK9" s="24"/>
+      <c r="AL9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO9" s="24"/>
+      <c r="AP9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS9" s="24"/>
+      <c r="AT9" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="24"/>
+      <c r="R10" t="s">
+        <v>84</v>
+      </c>
+      <c r="T10" t="s">
+        <v>13</v>
+      </c>
+      <c r="U10" s="24"/>
+      <c r="V10" t="s">
+        <v>84</v>
+      </c>
+      <c r="X10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="24"/>
+      <c r="Z10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC10" s="24"/>
+      <c r="AD10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG10" s="24"/>
+      <c r="AH10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK10" s="24"/>
+      <c r="AL10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO10" s="24"/>
+      <c r="AP10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS10" s="24"/>
+      <c r="AT10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" t="s">
+        <v>85</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="24"/>
+      <c r="R11" t="s">
+        <v>85</v>
+      </c>
+      <c r="T11" t="s">
+        <v>13</v>
+      </c>
+      <c r="U11" s="24"/>
+      <c r="V11" t="s">
+        <v>85</v>
+      </c>
+      <c r="X11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="24"/>
+      <c r="Z11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC11" s="24"/>
+      <c r="AD11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG11" s="24"/>
+      <c r="AH11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK11" s="24"/>
+      <c r="AL11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO11" s="24"/>
+      <c r="AP11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS11" s="24"/>
+      <c r="AT11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="24"/>
+      <c r="R12" t="s">
+        <v>86</v>
+      </c>
+      <c r="T12" t="s">
+        <v>13</v>
+      </c>
+      <c r="U12" s="24"/>
+      <c r="V12" t="s">
+        <v>86</v>
+      </c>
+      <c r="X12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y12" s="24"/>
+      <c r="Z12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="24"/>
+      <c r="AD12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG12" s="24"/>
+      <c r="AH12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK12" s="24"/>
+      <c r="AL12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO12" s="24"/>
+      <c r="AP12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS12" s="24"/>
+      <c r="AT12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="24"/>
+      <c r="J13" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="24"/>
+      <c r="N13" t="s">
+        <v>87</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="24"/>
+      <c r="R13" t="s">
+        <v>87</v>
+      </c>
+      <c r="T13" t="s">
+        <v>13</v>
+      </c>
+      <c r="U13" s="24"/>
+      <c r="V13" t="s">
+        <v>87</v>
+      </c>
+      <c r="X13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="24"/>
+      <c r="Z13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC13" s="24"/>
+      <c r="AD13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG13" s="24"/>
+      <c r="AH13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK13" s="24"/>
+      <c r="AL13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO13" s="24"/>
+      <c r="AP13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS13" s="24"/>
+      <c r="AT13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C2:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="24"/>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" s="24"/>
+      <c r="V14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="24"/>
+      <c r="Z14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC14" s="24"/>
+      <c r="AD14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG14" s="24"/>
+      <c r="AH14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK14" s="24"/>
+      <c r="AL14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="24"/>
+      <c r="AP14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS14" s="24"/>
+      <c r="AT14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="E15" s="24"/>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="24"/>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="24"/>
+      <c r="R15" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>13</v>
+      </c>
+      <c r="U15" s="24"/>
+      <c r="V15" t="s">
+        <v>3</v>
+      </c>
+      <c r="X15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="24"/>
+      <c r="Z15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="24"/>
+      <c r="AD15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG15" s="24"/>
+      <c r="AH15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK15" s="24"/>
+      <c r="AL15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO15" s="24"/>
+      <c r="AP15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS15" s="24"/>
+      <c r="AT15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="24"/>
+      <c r="J16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="24"/>
+      <c r="R16" t="s">
+        <v>2</v>
+      </c>
+      <c r="T16" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" s="24"/>
+      <c r="V16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y16" s="24"/>
+      <c r="Z16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC16" s="24"/>
+      <c r="AD16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG16" s="24"/>
+      <c r="AH16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK16" s="24"/>
+      <c r="AL16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO16" s="24"/>
+      <c r="AP16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS16" s="24"/>
+      <c r="AT16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="24"/>
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="24"/>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" t="s">
+        <v>13</v>
+      </c>
+      <c r="U17" s="24"/>
+      <c r="V17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="24"/>
+      <c r="Z17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC17" s="24"/>
+      <c r="AD17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG17" s="24"/>
+      <c r="AH17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK17" s="24"/>
+      <c r="AL17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO17" s="24"/>
+      <c r="AP17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS17" s="24"/>
+      <c r="AT17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18">
+        <f>C14+C16+C17</f>
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="24"/>
+      <c r="N18" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="24"/>
+      <c r="R18" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" t="s">
+        <v>13</v>
+      </c>
+      <c r="U18" s="24"/>
+      <c r="V18" t="s">
+        <v>34</v>
+      </c>
+      <c r="X18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y18" s="24"/>
+      <c r="Z18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC18" s="24"/>
+      <c r="AD18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG18" s="24"/>
+      <c r="AH18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK18" s="24"/>
+      <c r="AL18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO18" s="24"/>
+      <c r="AP18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS18" s="24"/>
+      <c r="AT18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="E19" s="24"/>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="24"/>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="24"/>
+      <c r="N19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19" s="24"/>
+      <c r="R19" t="s">
+        <v>33</v>
+      </c>
+      <c r="T19" t="s">
+        <v>13</v>
+      </c>
+      <c r="U19" s="24"/>
+      <c r="V19" t="s">
+        <v>33</v>
+      </c>
+      <c r="X19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y19" s="24"/>
+      <c r="Z19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC19" s="24"/>
+      <c r="AD19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG19" s="24"/>
+      <c r="AH19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK19" s="24"/>
+      <c r="AL19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO19" s="24"/>
+      <c r="AP19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS19" s="24"/>
+      <c r="AT19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="24"/>
+      <c r="J20" t="s">
+        <v>88</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="24"/>
+      <c r="N20" t="s">
+        <v>88</v>
+      </c>
+      <c r="P20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="24"/>
+      <c r="R20" t="s">
+        <v>88</v>
+      </c>
+      <c r="T20" t="s">
+        <v>13</v>
+      </c>
+      <c r="U20" s="24"/>
+      <c r="V20" t="s">
+        <v>88</v>
+      </c>
+      <c r="X20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y20" s="24"/>
+      <c r="Z20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="24"/>
+      <c r="AD20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG20" s="24"/>
+      <c r="AH20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK20" s="24"/>
+      <c r="AL20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO20" s="24"/>
+      <c r="AP20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS20" s="24"/>
+      <c r="AT20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="24"/>
+      <c r="N21" t="s">
+        <v>46</v>
+      </c>
+      <c r="P21" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="24"/>
+      <c r="R21" t="s">
+        <v>46</v>
+      </c>
+      <c r="T21" t="s">
+        <v>13</v>
+      </c>
+      <c r="U21" s="24"/>
+      <c r="V21" t="s">
+        <v>46</v>
+      </c>
+      <c r="X21" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y21" s="24"/>
+      <c r="Z21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC21" s="24"/>
+      <c r="AD21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG21" s="24"/>
+      <c r="AH21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK21" s="24"/>
+      <c r="AL21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO21" s="24"/>
+      <c r="AP21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS21" s="24"/>
+      <c r="AT21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="24"/>
+      <c r="J22" t="s">
+        <v>89</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" t="s">
+        <v>89</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q22" s="24"/>
+      <c r="R22" t="s">
+        <v>89</v>
+      </c>
+      <c r="T22" t="s">
+        <v>13</v>
+      </c>
+      <c r="U22" s="24"/>
+      <c r="V22" t="s">
+        <v>89</v>
+      </c>
+      <c r="X22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y22" s="24"/>
+      <c r="Z22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC22" s="24"/>
+      <c r="AD22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG22" s="24"/>
+      <c r="AH22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK22" s="24"/>
+      <c r="AL22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO22" s="24"/>
+      <c r="AP22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS22" s="24"/>
+      <c r="AT22" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23">
+        <f>C18+C20+C21+C22</f>
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="24"/>
+      <c r="J23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="24"/>
+      <c r="N23" t="s">
+        <v>90</v>
+      </c>
+      <c r="P23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="24"/>
+      <c r="R23" t="s">
+        <v>90</v>
+      </c>
+      <c r="T23" t="s">
+        <v>13</v>
+      </c>
+      <c r="U23" s="24"/>
+      <c r="V23" t="s">
+        <v>90</v>
+      </c>
+      <c r="X23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y23" s="24"/>
+      <c r="Z23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC23" s="24"/>
+      <c r="AD23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG23" s="24"/>
+      <c r="AH23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK23" s="24"/>
+      <c r="AL23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO23" s="24"/>
+      <c r="AP23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS23" s="24"/>
+      <c r="AT23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="E24" s="24"/>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="24"/>
+      <c r="J24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="24"/>
+      <c r="N24" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24" s="24"/>
+      <c r="R24" t="s">
+        <v>9</v>
+      </c>
+      <c r="T24" t="s">
+        <v>13</v>
+      </c>
+      <c r="U24" s="24"/>
+      <c r="V24" t="s">
+        <v>9</v>
+      </c>
+      <c r="X24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y24" s="24"/>
+      <c r="Z24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC24" s="24"/>
+      <c r="AD24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG24" s="24"/>
+      <c r="AH24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK24" s="24"/>
+      <c r="AL24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO24" s="24"/>
+      <c r="AP24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR24" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS24" s="24"/>
+      <c r="AT24" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="E25" s="24"/>
+      <c r="F25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="24"/>
+      <c r="J25" t="s">
+        <v>91</v>
+      </c>
+      <c r="L25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" s="24"/>
+      <c r="N25" t="s">
+        <v>91</v>
+      </c>
+      <c r="P25" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="24"/>
+      <c r="R25" t="s">
+        <v>91</v>
+      </c>
+      <c r="T25" t="s">
+        <v>13</v>
+      </c>
+      <c r="U25" s="24"/>
+      <c r="V25" t="s">
+        <v>91</v>
+      </c>
+      <c r="X25" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y25" s="24"/>
+      <c r="Z25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC25" s="24"/>
+      <c r="AD25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG25" s="24"/>
+      <c r="AH25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK25" s="24"/>
+      <c r="AL25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO25" s="24"/>
+      <c r="AP25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS25" s="24"/>
+      <c r="AT25" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12">
+        <f>C3+C4+C5+C6+C7+C8</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="13">
+        <f>G14+G15+G16+G17+G18+G19</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="13">
+        <f>C18-F28</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="13">
+        <f>C20+C21-F29</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="14">
+        <f>C16</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="13">
+        <f>C13</f>
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="13">
+        <f>C17</f>
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="13">
+        <f>G4</f>
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="13">
+        <f>G21</f>
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5F06E4-4B71-4DD5-A2F8-F472E18DC771}">
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -12919,69 +16536,69 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="18"/>
       <c r="D1" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="28"/>
       <c r="F1" s="18"/>
       <c r="G1" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="27"/>
       <c r="I1" s="18"/>
       <c r="J1" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K1" s="26"/>
       <c r="L1" s="18"/>
       <c r="M1" s="27" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N1" s="27"/>
       <c r="O1" s="18"/>
       <c r="P1" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="26"/>
       <c r="R1" s="18"/>
       <c r="S1" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T1" s="27"/>
       <c r="U1" s="18"/>
       <c r="V1" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W1" s="26"/>
       <c r="X1" s="18"/>
       <c r="Y1" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z1" s="27"/>
       <c r="AA1" s="18"/>
       <c r="AB1" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC1" s="26"/>
       <c r="AD1" s="18"/>
       <c r="AE1" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AF1" s="27"/>
       <c r="AG1" s="18"/>
       <c r="AH1" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AI1" s="26"/>
       <c r="AJ1" s="18"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="20">
         <f>'Apollo 5'!F28</f>
@@ -13079,7 +16696,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="20">
         <f>'Apollo 5'!F29</f>
@@ -13270,7 +16887,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="20">
         <f>'Apollo 5'!F30</f>
@@ -13368,7 +16985,7 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" s="20">
         <f>'Apollo 5'!F31</f>
@@ -13466,7 +17083,7 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="20">
         <f>'Apollo 5'!G13/2</f>
@@ -13474,7 +17091,7 @@
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="20">
         <f>'Apollo 7'!G21/2</f>
@@ -13564,7 +17181,7 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B8" s="20">
         <f>'Apollo 5'!G13/2</f>
@@ -13572,7 +17189,7 @@
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="20">
         <f>'Apollo 7'!G21/2</f>
@@ -13662,7 +17279,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9"/>
       <c r="E9" s="21"/>
@@ -13836,7 +17453,7 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="str">
@@ -14054,7 +17671,7 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" ref="A11:A16" si="11">A7&amp;" "&amp;B7</f>
+        <f t="shared" ref="A15:A16" si="11">A7&amp;" "&amp;B7</f>
         <v>APSFMASS1 29.25</v>
       </c>
       <c r="C15"/>
@@ -14223,8 +17840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3AF703-9709-4902-BBAD-427EF3ACED08}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="A23:F25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17289,7 +20906,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23418,8 +27035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8F2989-E811-4229-822B-85C41BBD0FB6}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="A23:I28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26484,7 +30101,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29585,7 +33202,7 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D47" sqref="D46:D47"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32682,8 +36299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35784,7 +39401,7 @@
   <dimension ref="A1:BD41"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Skylab 1 masses
</commit_message>
<xml_diff>
--- a/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
+++ b/Doc/Project Apollo - NASSP/Saturn Masses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Orbiter2016 Beta\Doc\Project Apollo - NASSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC89749-DE31-4210-8970-D2E3798A348E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835D8721-DC13-4CBA-9EA6-EC339CC3EFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo 17" sheetId="11" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8545" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8547" uniqueCount="161">
   <si>
     <t>S-IC Stage Dry</t>
   </si>
@@ -528,6 +528,12 @@
   <si>
     <t>OWSMETSHLD</t>
   </si>
+  <si>
+    <t>PAYLOADSHROUD</t>
+  </si>
+  <si>
+    <t>Payload Shroud</t>
+  </si>
 </sst>
 </file>
 
@@ -739,13 +745,13 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12905,7 +12911,7 @@
   <dimension ref="A1:AB42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13244,6 +13250,15 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
+      <c r="Z6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA6">
+        <v>12701</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -14181,11 +14196,11 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="B33">
-        <f>AA3+AA4</f>
-        <v>22</v>
+        <f>AA6</f>
+        <v>12701</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>13</v>
@@ -16535,65 +16550,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="18"/>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="28"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="18"/>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="18"/>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="26"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="18"/>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="27"/>
+      <c r="N1" s="28"/>
       <c r="O1" s="18"/>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="26"/>
+      <c r="Q1" s="27"/>
       <c r="R1" s="18"/>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="27"/>
+      <c r="T1" s="28"/>
       <c r="U1" s="18"/>
-      <c r="V1" s="26" t="s">
+      <c r="V1" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="26"/>
+      <c r="W1" s="27"/>
       <c r="X1" s="18"/>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="27"/>
+      <c r="Z1" s="28"/>
       <c r="AA1" s="18"/>
-      <c r="AB1" s="26" t="s">
+      <c r="AB1" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="AC1" s="26"/>
+      <c r="AC1" s="27"/>
       <c r="AD1" s="18"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AE1" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" s="27"/>
+      <c r="AF1" s="28"/>
       <c r="AG1" s="18"/>
-      <c r="AH1" s="26" t="s">
+      <c r="AH1" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="AI1" s="26"/>
+      <c r="AI1" s="27"/>
       <c r="AJ1" s="18"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -17817,11 +17832,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="D1:E1"/>
@@ -17829,6 +17839,11 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39400,7 +39415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BD41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>